<commit_message>
ValueSet Creation for DocumentReference.type and Rules modification b086db36a38746f0cae8e238c882bb4cd2d4dd84
</commit_message>
<xml_diff>
--- a/issues96/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/issues96/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-03T15:04:53+00:00</t>
+    <t>2024-04-04T12:58:54+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -66,7 +66,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>ANS (https://esante.gouv.fr)</t>
   </si>
   <si>
     <t>Jurisdiction</t>

</xml_diff>

<commit_message>
clear QA + fix cardinalities problem
Clear QA :
Ajout d'une description pour les exemples
Ajout d'un titre pour les ressources
Suppression des espaces au début et à la fin des chaines de caractères
Modification Règle de gestions pour gérer les attributs répétables plus proprement

Modification cardinalités :
ESMSDocumentReference.type.coding passe à 1..1 pour évitr plusieurs coding sous un CodeableConcept
SDOTask.input[modePriseCharge].coding passe à 1..1 pour éviter plusieurs coding sous un codeableConcept 5a048b60bc17e59a4997e6d0ca84604a11722ef8
</commit_message>
<xml_diff>
--- a/issues96/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/issues96/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
   <si>
     <t>Property</t>
   </si>
@@ -51,10 +51,13 @@
     <t>Experimental</t>
   </si>
   <si>
+    <t>false</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-05T07:48:28+00:00</t>
+    <t>2024-04-08T12:44:22+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -102,9 +105,6 @@
     <t>Compositional</t>
   </si>
   <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>Version Needed?</t>
   </si>
   <si>
@@ -141,7 +141,7 @@
     <t>idNat_Struct</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifiant de l'ESMS accueillant l'individu en situation de handicap. Cet identifiant est obtenu par la concaténation du type d'identifiant national de structure (provenant de la nomenclature TRE_G07-TypeIdentifiantStructure) et de l'identifiant de la structure: ** 1 + N° FINESS (entité juridique et entité géographique indéterminées);** 3 + N° SIRET </t>
+    <t>Identifiant de l'ESMS accueillant l'individu en situation de handicap. Cet identifiant est obtenu par la concaténation du type d'identifiant national de structure (provenant de la nomenclature TRE_G07-TypeIdentifiantStructure) et de l'identifiant de la structure: ** 1 + N° FINESS (entité juridique et entité géographique indéterminées);** 3 + N° SIRET</t>
   </si>
   <si>
     <t>nomESMS</t>
@@ -417,7 +417,9 @@
       <c r="A5" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
@@ -431,86 +433,88 @@
       <c r="A7" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" t="s" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">

</xml_diff>